<commit_message>
progress in random method (evolutionary): use initial solution provided by nearest neighbor and then mutates the solution and compare with the current solution; best solution (min Wmax) is conserved and the other is discarded.
</commit_message>
<xml_diff>
--- a/constructive_method/reports/report.xlsx
+++ b/constructive_method/reports/report.xlsx
@@ -512,7 +512,7 @@
         <v>504.56</v>
       </c>
       <c r="H2" t="n">
-        <v>0.009101629257202148</v>
+        <v>0.00300288200378418</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>513.7</v>
+        <v>515.53</v>
       </c>
       <c r="D3" t="n">
-        <v>511.99</v>
+        <v>514.91</v>
       </c>
       <c r="E3" t="n">
-        <v>1.71</v>
+        <v>0.62</v>
       </c>
       <c r="F3" t="n">
-        <v>1025.69</v>
+        <v>1030.44</v>
       </c>
       <c r="G3" t="n">
-        <v>512.85</v>
+        <v>515.22</v>
       </c>
       <c r="H3" t="n">
-        <v>1.645229816436768</v>
+        <v>1.626104116439819</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>546.3099999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0156247615814209</v>
+        <v>0.002505064010620117</v>
       </c>
     </row>
     <row r="5">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>643.21</v>
+        <v>648.26</v>
       </c>
       <c r="D5" t="n">
-        <v>484.85</v>
+        <v>480.69</v>
       </c>
       <c r="E5" t="n">
-        <v>158.36</v>
+        <v>167.56</v>
       </c>
       <c r="F5" t="n">
-        <v>1128.06</v>
+        <v>1128.95</v>
       </c>
       <c r="G5" t="n">
-        <v>564.03</v>
+        <v>564.47</v>
       </c>
       <c r="H5" t="n">
-        <v>1.706416845321655</v>
+        <v>1.693790912628174</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01088953018188477</v>
+        <v>0.006505250930786133</v>
       </c>
     </row>
     <row r="7">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>554.65</v>
+        <v>555.7</v>
       </c>
       <c r="D7" t="n">
-        <v>551.54</v>
+        <v>548.53</v>
       </c>
       <c r="E7" t="n">
-        <v>3.11</v>
+        <v>7.17</v>
       </c>
       <c r="F7" t="n">
-        <v>1658.27</v>
+        <v>1653.52</v>
       </c>
       <c r="G7" t="n">
-        <v>552.76</v>
+        <v>551.17</v>
       </c>
       <c r="H7" t="n">
-        <v>3.723294496536255</v>
+        <v>3.580146789550781</v>
       </c>
     </row>
     <row r="8">
@@ -692,7 +692,7 @@
         <v>582.2</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01558709144592285</v>
+        <v>0.007514238357543945</v>
       </c>
     </row>
     <row r="9">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>647.8099999999999</v>
+        <v>644.21</v>
       </c>
       <c r="D9" t="n">
-        <v>511.62</v>
+        <v>508.83</v>
       </c>
       <c r="E9" t="n">
-        <v>136.2</v>
+        <v>135.37</v>
       </c>
       <c r="F9" t="n">
-        <v>1795.15</v>
+        <v>1796.22</v>
       </c>
       <c r="G9" t="n">
-        <v>598.38</v>
+        <v>598.74</v>
       </c>
       <c r="H9" t="n">
-        <v>3.89091157913208</v>
+        <v>3.922915458679199</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01566910743713379</v>
+        <v>0.01050400733947754</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>542.6799999999999</v>
+        <v>541.97</v>
       </c>
       <c r="D11" t="n">
-        <v>529.17</v>
+        <v>523.75</v>
       </c>
       <c r="E11" t="n">
-        <v>13.52</v>
+        <v>18.22</v>
       </c>
       <c r="F11" t="n">
-        <v>2149.25</v>
+        <v>2141.73</v>
       </c>
       <c r="G11" t="n">
-        <v>537.3099999999999</v>
+        <v>535.4299999999999</v>
       </c>
       <c r="H11" t="n">
-        <v>5.850036859512329</v>
+        <v>5.896767854690552</v>
       </c>
     </row>
     <row r="12">
@@ -812,7 +812,7 @@
         <v>564.01</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01562738418579102</v>
+        <v>0.01150727272033691</v>
       </c>
     </row>
     <row r="13">
@@ -827,22 +827,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>679.96</v>
+        <v>696.2</v>
       </c>
       <c r="D13" t="n">
-        <v>452.27</v>
+        <v>467.39</v>
       </c>
       <c r="E13" t="n">
-        <v>227.69</v>
+        <v>228.81</v>
       </c>
       <c r="F13" t="n">
-        <v>2337.28</v>
+        <v>2328.68</v>
       </c>
       <c r="G13" t="n">
-        <v>584.3200000000001</v>
+        <v>582.17</v>
       </c>
       <c r="H13" t="n">
-        <v>6.323891401290894</v>
+        <v>6.262850284576416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress: find bks, comparison table and statistical analysis working
</commit_message>
<xml_diff>
--- a/constructive_method/reports/report.xlsx
+++ b/constructive_method/reports/report.xlsx
@@ -512,7 +512,7 @@
         <v>504.56</v>
       </c>
       <c r="H2" t="n">
-        <v>0.00300288200378418</v>
+        <v>0.003000259399414062</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>515.53</v>
+        <v>514.34</v>
       </c>
       <c r="D3" t="n">
-        <v>514.91</v>
+        <v>512.67</v>
       </c>
       <c r="E3" t="n">
-        <v>0.62</v>
+        <v>1.67</v>
       </c>
       <c r="F3" t="n">
-        <v>1030.44</v>
+        <v>1027.01</v>
       </c>
       <c r="G3" t="n">
-        <v>515.22</v>
+        <v>513.5</v>
       </c>
       <c r="H3" t="n">
-        <v>1.626104116439819</v>
+        <v>1.598640203475952</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>546.3099999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.002505064010620117</v>
+        <v>0.003998994827270508</v>
       </c>
     </row>
     <row r="5">
@@ -587,22 +587,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>648.26</v>
+        <v>627.89</v>
       </c>
       <c r="D5" t="n">
-        <v>480.69</v>
+        <v>491.7</v>
       </c>
       <c r="E5" t="n">
-        <v>167.56</v>
+        <v>136.19</v>
       </c>
       <c r="F5" t="n">
-        <v>1128.95</v>
+        <v>1119.59</v>
       </c>
       <c r="G5" t="n">
-        <v>564.47</v>
+        <v>559.8</v>
       </c>
       <c r="H5" t="n">
-        <v>1.693790912628174</v>
+        <v>1.647355318069458</v>
       </c>
     </row>
     <row r="6">
@@ -632,7 +632,7 @@
         <v>540.9400000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.006505250930786133</v>
+        <v>0.007999897003173828</v>
       </c>
     </row>
     <row r="7">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>555.7</v>
+        <v>553.34</v>
       </c>
       <c r="D7" t="n">
-        <v>548.53</v>
+        <v>551.22</v>
       </c>
       <c r="E7" t="n">
-        <v>7.17</v>
+        <v>2.11</v>
       </c>
       <c r="F7" t="n">
-        <v>1653.52</v>
+        <v>1656.81</v>
       </c>
       <c r="G7" t="n">
-        <v>551.17</v>
+        <v>552.27</v>
       </c>
       <c r="H7" t="n">
-        <v>3.580146789550781</v>
+        <v>3.590090274810791</v>
       </c>
     </row>
     <row r="8">
@@ -692,7 +692,7 @@
         <v>582.2</v>
       </c>
       <c r="H8" t="n">
-        <v>0.007514238357543945</v>
+        <v>0.008063077926635742</v>
       </c>
     </row>
     <row r="9">
@@ -707,22 +707,22 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>644.21</v>
+        <v>640.11</v>
       </c>
       <c r="D9" t="n">
-        <v>508.83</v>
+        <v>513.79</v>
       </c>
       <c r="E9" t="n">
-        <v>135.37</v>
+        <v>126.32</v>
       </c>
       <c r="F9" t="n">
-        <v>1796.22</v>
+        <v>1792.56</v>
       </c>
       <c r="G9" t="n">
-        <v>598.74</v>
+        <v>597.52</v>
       </c>
       <c r="H9" t="n">
-        <v>3.922915458679199</v>
+        <v>3.861264705657959</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         <v>521.63</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01050400733947754</v>
+        <v>0.01200008392333984</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +767,22 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>541.97</v>
+        <v>543.09</v>
       </c>
       <c r="D11" t="n">
-        <v>523.75</v>
+        <v>515.6900000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>18.22</v>
+        <v>27.4</v>
       </c>
       <c r="F11" t="n">
-        <v>2141.73</v>
+        <v>2139.9</v>
       </c>
       <c r="G11" t="n">
-        <v>535.4299999999999</v>
+        <v>534.97</v>
       </c>
       <c r="H11" t="n">
-        <v>5.896767854690552</v>
+        <v>6.09990930557251</v>
       </c>
     </row>
     <row r="12">
@@ -812,7 +812,7 @@
         <v>564.01</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01150727272033691</v>
+        <v>0.01099920272827148</v>
       </c>
     </row>
     <row r="13">
@@ -827,22 +827,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>696.2</v>
+        <v>701.87</v>
       </c>
       <c r="D13" t="n">
-        <v>467.39</v>
+        <v>465.73</v>
       </c>
       <c r="E13" t="n">
-        <v>228.81</v>
+        <v>236.14</v>
       </c>
       <c r="F13" t="n">
-        <v>2328.68</v>
+        <v>2332.26</v>
       </c>
       <c r="G13" t="n">
-        <v>582.17</v>
+        <v>583.0599999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>6.262850284576416</v>
+        <v>6.773151874542236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>